<commit_message>
zaw - Wrote DB Tables & Basic Doc
</commit_message>
<xml_diff>
--- a/documentation/00_要件定義/01_要件定義書.xlsx
+++ b/documentation/00_要件定義/01_要件定義書.xlsx
@@ -23,7 +23,7 @@
     <t>目的</t>
   </si>
   <si>
-    <t>管理者が本をサーバー上にアプロードし、ユーザー側でウェブ上本を買えるサービスシステム開発に関する要件定義書になります。</t>
+    <t>管理者が本をサーバー上にアプロードし、ユーザー側でウェブ上本を買えるサービスに関する要件定義書になります。</t>
   </si>
   <si>
     <t>概要</t>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="SimSun"/>
+        <charset val="134"/>
+      </rPr>
       <t>登録</t>
     </r>
     <r>
@@ -140,6 +146,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="MS Gothic"/>
+        <charset val="134"/>
+      </rPr>
       <t>システム</t>
     </r>
     <r>
@@ -306,10 +318,10 @@
     <t>６。注文リスト画面</t>
   </si>
   <si>
-    <t>７．配送先住所画面</t>
-  </si>
-  <si>
-    <t>８．請求先住所画面</t>
+    <t>７．配送先画面</t>
+  </si>
+  <si>
+    <t>８．請求先画面</t>
   </si>
   <si>
     <t>９．ショッピングカート画面</t>
@@ -368,12 +380,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,14 +437,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,13 +458,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -469,13 +474,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -531,6 +529,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -546,7 +551,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,13 +572,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,6 +589,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -596,13 +661,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,13 +703,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,13 +745,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,115 +757,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,15 +820,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -849,6 +845,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -863,17 +874,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -915,152 +920,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1083,7 +1088,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1406,8 +1410,8 @@
   <sheetPr/>
   <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1629,7 +1633,7 @@
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1639,22 +1643,22 @@
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="16" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="17"/>
+      <c r="A58" s="16"/>
     </row>
     <row r="59" ht="21" spans="1:1">
       <c r="A59" s="10" t="s">

</xml_diff>